<commit_message>
feat: add runtime comparision for heuristic algos
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069C0E9C-C81D-5149-AEDA-598DED37643E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF889BE-608D-9C44-A0E8-9A8DC38502C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4800" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{75212AE2-A3F9-034E-9D2E-443F9B0F6379}"/>
+    <workbookView xWindow="-4260" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{75212AE2-A3F9-034E-9D2E-443F9B0F6379}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
     </textPr>
   </connection>
   <connection id="6" xr16:uid="{FBCC0161-8876-464A-876C-CD34D003F0BC}" name="result_greedy" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_greedy.txt" tab="0" space="1" consecutive="1">
+    <textPr sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_greedy.txt" tab="0" space="1" consecutive="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -95,7 +95,7 @@
     </textPr>
   </connection>
   <connection id="7" xr16:uid="{CCB4EA36-AB10-9644-96B6-0372920FC633}" name="result_mst" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_mst.txt" tab="0" space="1" consecutive="1">
+    <textPr sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_mst.txt" tab="0" space="1" consecutive="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -1467,15 +1467,6 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-3C35-CA42-A871-90C9AD6AD040}"/>
@@ -1500,15 +1491,6 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000D-3C35-CA42-A871-90C9AD6AD040}"/>
@@ -1533,15 +1515,6 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000F-3C35-CA42-A871-90C9AD6AD040}"/>
@@ -1566,15 +1539,6 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000011-3C35-CA42-A871-90C9AD6AD040}"/>
@@ -1599,15 +1563,6 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000013-3C35-CA42-A871-90C9AD6AD040}"/>
@@ -1632,15 +1587,6 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000015-3C35-CA42-A871-90C9AD6AD040}"/>
@@ -1665,15 +1611,6 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000017-3C35-CA42-A871-90C9AD6AD040}"/>
@@ -1698,15 +1635,6 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000019-3C35-CA42-A871-90C9AD6AD040}"/>
@@ -2893,6 +2821,982 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Runtime</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Comparison (Log scale base 10)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Dynamic Programming</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-414D-594E-8F18-81DB34697FEC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-414D-594E-8F18-81DB34697FEC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-414D-594E-8F18-81DB34697FEC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$13:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$13:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>3.2562599517405003E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5354180727154E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0225009433925099E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.2733400631695904E-5</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>2.0665838383138101E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>4.36891580466181E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>1.07114161364734E-3</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>2.4844876141287301E-3</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>5.9574958169832798E-3</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>1.4177412388380601E-2</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>3.40078002074733E-2</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>7.7598812500946204E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.178692003979813</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.41521392923314099</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.98155113327084098</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.2970354792894701</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>5.6326177082140898</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>14.5183411833015</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>34.6804867958882</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-414D-594E-8F18-81DB34697FEC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Greedy</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$1:$P$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$1:$S$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>3.5825002123601699E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4354098897892903E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.17083991831168E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6779201764147702E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9858299714978703E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.6095800644252399E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.22289978107437E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.7079103135038101E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.8720702226273702E-5</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>1.0771249944809801E-4</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>1.4403740351554001E-4</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>1.5826250164536701E-4</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>1.67962297564372E-4</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>1.8422069842927101E-4</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>1.91808499221224E-4</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>2.1978720033075599E-4</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>2.2655820066574901E-4</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>9.8596230236580595E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-414D-594E-8F18-81DB34697FEC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Minimum spanning tree</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$21:$P$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$21:$S$38</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>4.6187700354494102E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3058401681482698E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4366501970216602E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8300101479981097E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4966602076310602E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0300201585050602E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.4704300893936295E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.80832003126852E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.2270900020375796E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.1658398266881696E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.3754001136403496E-5</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>1.06099997356068E-4</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>1.1902499827556299E-4</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>1.3036659802310099E-4</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>1.47987499076407E-4</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>1.6299589915433899E-4</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>1.7460410308558401E-4</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>2.1869589836569499E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-414D-594E-8F18-81DB34697FEC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="390205664"/>
+        <c:axId val="390244464"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="390205664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Cities</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="390244464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="390244464"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Runtime (second)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="390205664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3013,6 +3917,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4046,6 +4990,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4675,11 +6135,49 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>430449</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>124581</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C959C5B5-7B9E-1C48-9397-855654895839}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_mst" connectionId="7" xr16:uid="{D6160FED-F641-B34B-BFBC-438099521667}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_br" connectionId="1" xr16:uid="{D13C840A-1D9F-8547-9FCE-E9EBA5D372AF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4687,23 +6185,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_dp" connectionId="3" xr16:uid="{A38A6EA9-0153-0D4A-9803-DC447E61790C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_dp_3" connectionId="4" xr16:uid="{431A5A0A-0D00-6746-A729-0C8671FDF2E8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_dp_2" connectionId="5" xr16:uid="{448F1A0E-9594-1D47-ADA1-8FA9959D8C52}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_br_2" connectionId="2" xr16:uid="{2968DE33-C909-9B4F-9608-A1CC59D8E9A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_br" connectionId="1" xr16:uid="{D13C840A-1D9F-8547-9FCE-E9EBA5D372AF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_dp" connectionId="3" xr16:uid="{A38A6EA9-0153-0D4A-9803-DC447E61790C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_mst" connectionId="7" xr16:uid="{D6160FED-F641-B34B-BFBC-438099521667}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5005,8 +6503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB42E8F-E18A-D64A-A94C-602C99A3A6CC}">
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="132" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="AD12" sqref="AD12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="U47" sqref="U47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix: add missing data
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF889BE-608D-9C44-A0E8-9A8DC38502C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C878F8-501D-0B47-9D72-59A20A413836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4260" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{75212AE2-A3F9-034E-9D2E-443F9B0F6379}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27620" windowHeight="17500" xr2:uid="{75212AE2-A3F9-034E-9D2E-443F9B0F6379}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
     <definedName name="result_dp" localSheetId="0">Sheet1!$A$13:$B$22</definedName>
     <definedName name="result_dp_2" localSheetId="0">Sheet1!$A$13:$B$22</definedName>
     <definedName name="result_dp_3" localSheetId="0">Sheet1!$A$23:$B$31</definedName>
-    <definedName name="result_greedy" localSheetId="0">Sheet1!$P$1:$Q$18</definedName>
-    <definedName name="result_mst" localSheetId="0">Sheet1!$P$21:$Q$38</definedName>
+    <definedName name="result_greedy" localSheetId="0">Sheet1!$P$1:$Q$19</definedName>
+    <definedName name="result_mst" localSheetId="0">Sheet1!$P$21:$Q$39</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -2175,10 +2175,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$1:$P$18</c:f>
+              <c:f>Sheet1!$P$1:$P$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -2231,6 +2231,9 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
@@ -2238,10 +2241,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$1:$Q$18</c:f>
+              <c:f>Sheet1!$Q$1:$Q$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2294,6 +2297,9 @@
                   <c:v>0.36569806706369301</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0.55610751928873203</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0.48313867179154701</c:v>
                 </c:pt>
               </c:numCache>
@@ -2352,10 +2358,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$21:$P$38</c:f>
+              <c:f>Sheet1!$P$21:$P$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -2408,6 +2414,9 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
@@ -2415,10 +2424,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$21:$Q$38</c:f>
+              <c:f>Sheet1!$Q$21:$Q$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2471,6 +2480,9 @@
                   <c:v>1.1675024965740799</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>1.34038524510091</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>1.2346367360332</c:v>
                 </c:pt>
               </c:numCache>
@@ -3174,10 +3186,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$1:$P$18</c:f>
+              <c:f>Sheet1!$P$1:$P$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -3230,6 +3242,9 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
@@ -3237,10 +3252,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$S$1:$S$18</c:f>
+              <c:f>Sheet1!$S$1:$S$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>3.5825002123601699E-5</c:v>
                 </c:pt>
@@ -3293,6 +3308,9 @@
                   <c:v>2.2655820066574901E-4</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
+                  <c:v>3.6107909982092598E-4</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
                   <c:v>9.8596230236580595E-4</c:v>
                 </c:pt>
               </c:numCache>
@@ -3337,10 +3355,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$21:$P$38</c:f>
+              <c:f>Sheet1!$P$21:$P$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -3393,6 +3411,9 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
@@ -3400,10 +3421,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$S$21:$S$38</c:f>
+              <c:f>Sheet1!$S$21:$S$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>4.6187700354494102E-5</c:v>
                 </c:pt>
@@ -3456,6 +3477,9 @@
                   <c:v>1.7460410308558401E-4</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
+                  <c:v>1.90300005488097E-4</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
                   <c:v>2.1869589836569499E-4</c:v>
                 </c:pt>
               </c:numCache>
@@ -6177,7 +6201,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_br" connectionId="1" xr16:uid="{D13C840A-1D9F-8547-9FCE-E9EBA5D372AF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_br_2" connectionId="2" xr16:uid="{2968DE33-C909-9B4F-9608-A1CC59D8E9A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6185,23 +6209,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_mst" connectionId="7" xr16:uid="{D6160FED-F641-B34B-BFBC-438099521667}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_dp" connectionId="3" xr16:uid="{A38A6EA9-0153-0D4A-9803-DC447E61790C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_dp_3" connectionId="4" xr16:uid="{431A5A0A-0D00-6746-A729-0C8671FDF2E8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_dp_2" connectionId="5" xr16:uid="{448F1A0E-9594-1D47-ADA1-8FA9959D8C52}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_br_2" connectionId="2" xr16:uid="{2968DE33-C909-9B4F-9608-A1CC59D8E9A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_mst" connectionId="7" xr16:uid="{D6160FED-F641-B34B-BFBC-438099521667}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_br" connectionId="1" xr16:uid="{D13C840A-1D9F-8547-9FCE-E9EBA5D372AF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6503,8 +6527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB42E8F-E18A-D64A-A94C-602C99A3A6CC}">
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="U47" sqref="U47"/>
+    <sheetView tabSelected="1" topLeftCell="C24" zoomScale="75" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6513,7 +6537,7 @@
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
     <col min="4" max="4" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" customWidth="1"/>
     <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -6803,13 +6827,13 @@
         <v>4.36891580466181E-4</v>
       </c>
       <c r="P18">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q18">
-        <v>0.48313867179154701</v>
+        <v>0.55610751928873203</v>
       </c>
       <c r="S18">
-        <v>9.8596230236580595E-4</v>
+        <v>3.6107909982092598E-4</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
@@ -6819,6 +6843,15 @@
       <c r="B19">
         <v>1.07114161364734E-3</v>
       </c>
+      <c r="P19">
+        <v>21</v>
+      </c>
+      <c r="Q19">
+        <v>0.48313867179154701</v>
+      </c>
+      <c r="S19">
+        <v>9.8596230236580595E-4</v>
+      </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -7084,17 +7117,26 @@
     <row r="38" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B38" s="1"/>
       <c r="P38">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q38">
-        <v>1.2346367360332</v>
+        <v>1.34038524510091</v>
       </c>
       <c r="S38">
-        <v>2.1869589836569499E-4</v>
+        <v>1.90300005488097E-4</v>
       </c>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
+      <c r="P39">
+        <v>21</v>
+      </c>
+      <c r="Q39">
+        <v>1.2346367360332</v>
+      </c>
+      <c r="S39">
+        <v>2.1869589836569499E-4</v>
+      </c>
       <c r="W39" s="2"/>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: update and improve scatter plots
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C878F8-501D-0B47-9D72-59A20A413836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933FA35E-2C52-4744-9BB4-2A391CAD9EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27620" windowHeight="17500" xr2:uid="{75212AE2-A3F9-034E-9D2E-443F9B0F6379}"/>
+    <workbookView xWindow="-4940" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{75212AE2-A3F9-034E-9D2E-443F9B0F6379}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="result_br" localSheetId="0">Sheet1!$A$1:$B$11</definedName>
-    <definedName name="result_br_2" localSheetId="0">Sheet1!$A$1:$B$10</definedName>
-    <definedName name="result_dp" localSheetId="0">Sheet1!$A$13:$B$22</definedName>
-    <definedName name="result_dp_2" localSheetId="0">Sheet1!$A$13:$B$22</definedName>
-    <definedName name="result_dp_3" localSheetId="0">Sheet1!$A$23:$B$31</definedName>
-    <definedName name="result_greedy" localSheetId="0">Sheet1!$P$1:$Q$19</definedName>
-    <definedName name="result_mst" localSheetId="0">Sheet1!$P$21:$Q$39</definedName>
+    <definedName name="result_br" localSheetId="0">Sheet1!$A$2:$B$12</definedName>
+    <definedName name="result_br_2" localSheetId="0">Sheet1!#REF!</definedName>
+    <definedName name="result_br_3" localSheetId="0">Sheet1!$A$2:$B$57</definedName>
+    <definedName name="result_dp" localSheetId="0">Sheet1!#REF!</definedName>
+    <definedName name="result_dp_2" localSheetId="0">Sheet1!#REF!</definedName>
+    <definedName name="result_dp_3" localSheetId="0">Sheet1!#REF!</definedName>
+    <definedName name="result_dp_4" localSheetId="0">Sheet1!$A$14:$B$32</definedName>
+    <definedName name="result_greedy_1" localSheetId="0">Sheet1!$P$2:$R$81</definedName>
+    <definedName name="result_mst_1" localSheetId="0">Sheet1!$AF$5:$AH$43</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -53,40 +55,32 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{B466C81D-FF8C-E345-A4E8-6C3D6D455CBC}" name="result_br11" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_br.txt" tab="0" space="1" consecutive="1">
-      <textFields count="2">
+  <connection id="2" xr16:uid="{31346737-7074-834E-ADE2-73C90860B480}" name="result_br1" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" firstRow="24" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_br.txt" tab="0" space="1" consecutive="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{1242D075-0E89-FF41-9648-400C2D170A11}" name="result_dp" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_dp.txt" tab="0" space="1" consecutive="1">
-      <textFields count="2">
+  <connection id="3" xr16:uid="{46BFB1C6-60FC-E246-856D-4A76B7E1C519}" name="result_dp3" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" firstRow="24" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_dp.txt" tab="0" space="1" consecutive="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{C7D65D8C-0D44-C646-930D-167593E67FC4}" name="result_dp1" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr firstRow="11" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_dp.txt" tab="0" space="1" consecutive="1">
-      <textFields count="2">
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="5" xr16:uid="{F62017FD-10CE-2840-AB0B-023E6B27761A}" name="result_dp2" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_dp.txt" tab="0" space="1" consecutive="1">
-      <textFields count="2">
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="6" xr16:uid="{FBCC0161-8876-464A-876C-CD34D003F0BC}" name="result_greedy" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_greedy.txt" tab="0" space="1" consecutive="1">
+  <connection id="4" xr16:uid="{E574AEC5-39E1-7045-BDA9-CB3CD0FBC749}" name="result_greedy1" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" firstRow="23" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_greedy.txt" tab="0" space="1" consecutive="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -94,8 +88,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" xr16:uid="{CCB4EA36-AB10-9644-96B6-0372920FC633}" name="result_mst" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_mst.txt" tab="0" space="1" consecutive="1">
+  <connection id="5" xr16:uid="{DC51D5A7-BA3B-3A49-8F6D-60E3001D7191}" name="result_mst1" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" firstRow="23" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_mst.txt" tab="0" space="1" consecutive="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -104,6 +98,20 @@
     </textPr>
   </connection>
 </connections>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>runtime</t>
+  </si>
+  <si>
+    <t>quality</t>
+  </si>
+  <si>
+    <t>Runtime</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -247,8 +255,123 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Exhaustive Search</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.2020428334362799E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2641708385199303E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1525000017136302E-5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>1.6029003134462901E-4</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>8.0889039963949396E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>5.5364337802166104E-3</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>4.4285878327791503E-2</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>0.40938890543067802</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>4.4097970754495996</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>52.464114895861101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000032-6F19-3047-B5C5-9E00AD6B912C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Dynamic Programming</c:v>
           </c:tx>
@@ -276,81 +399,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dPt>
-            <c:idx val="12"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000A-6F19-3047-B5C5-9E00AD6B912C}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="13"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-6F19-3047-B5C5-9E00AD6B912C}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="14"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000C-6F19-3047-B5C5-9E00AD6B912C}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$13:$A$31</c:f>
+              <c:f>Sheet1!$A$14:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -416,66 +467,66 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$B$31</c:f>
+              <c:f>Sheet1!$B$14:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>3.2562599517405003E-5</c:v>
+                  <c:v>3.8732078974135202E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5354180727154E-5</c:v>
+                  <c:v>3.9045728626661003E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0225009433925099E-5</c:v>
+                  <c:v>6.6032973700202993E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.2733400631695904E-5</c:v>
+                  <c:v>9.1826239950023594E-5</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>2.0665838383138101E-4</c:v>
+                  <c:v>1.8501331971492599E-4</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>4.36891580466181E-4</c:v>
+                  <c:v>4.3670004000887202E-4</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>1.07114161364734E-3</c:v>
+                  <c:v>1.07894792687147E-3</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>2.4844876141287301E-3</c:v>
+                  <c:v>2.6988179399631898E-3</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>5.9574958169832798E-3</c:v>
+                  <c:v>6.34287457796745E-3</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
-                  <c:v>1.4177412388380601E-2</c:v>
+                  <c:v>1.5447837053216E-2</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>3.40078002074733E-2</c:v>
+                  <c:v>3.4396914600511003E-2</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>7.7598812500946204E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.178692003979813</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.41521392923314099</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.98155113327084098</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.2970354792894701</c:v>
+                  <c:v>7.9342790392693097E-2</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>0.18683972923376099</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>0.43679219301848199</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>1.04754431002773</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>2.6486301862337802</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>5.6326177082140898</c:v>
+                  <c:v>6.5284631966572402</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>14.5183411833015</c:v>
+                  <c:v>16.096170290021099</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
-                  <c:v>34.6804867958882</c:v>
+                  <c:v>37.426206192138402</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -484,289 +535,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6F19-3047-B5C5-9E00AD6B912C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Exhaustive Search</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000A-63AB-1240-9E7B-CF4A7A8A9C96}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000C-63AB-1240-9E7B-CF4A7A8A9C96}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000E-63AB-1240-9E7B-CF4A7A8A9C96}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000010-63AB-1240-9E7B-CF4A7A8A9C96}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000012-63AB-1240-9E7B-CF4A7A8A9C96}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000014-63AB-1240-9E7B-CF4A7A8A9C96}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000016-63AB-1240-9E7B-CF4A7A8A9C96}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$1:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$1:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2.4425087030977E-5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.9650092367082802E-5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0141825340688202E-5</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>1.93704187404364E-4</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>9.3917112099006696E-4</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>5.4293875000439498E-3</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>4.2910470569040599E-2</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>0.39486829169327298</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>4.1375219418900002</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>47.450318979192502</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000032-6F19-3047-B5C5-9E00AD6B912C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1179,8 +947,123 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Exhaustive Search</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.2020428334362799E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2641708385199303E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1525000017136302E-5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>1.6029003134462901E-4</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>8.0889039963949396E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>5.5364337802166104E-3</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>4.4285878327791503E-2</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>0.40938890543067802</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>4.4097970754495996</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>52.464114895861101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001A-3C35-CA42-A871-90C9AD6AD040}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Dynamic Programming</c:v>
           </c:tx>
@@ -1208,81 +1091,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dPt>
-            <c:idx val="12"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000006-3C35-CA42-A871-90C9AD6AD040}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="13"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-3C35-CA42-A871-90C9AD6AD040}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="14"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000008-3C35-CA42-A871-90C9AD6AD040}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$13:$A$31</c:f>
+              <c:f>Sheet1!$A$14:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1348,66 +1159,66 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$B$31</c:f>
+              <c:f>Sheet1!$B$14:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>3.2562599517405003E-5</c:v>
+                  <c:v>3.8732078974135202E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5354180727154E-5</c:v>
+                  <c:v>3.9045728626661003E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0225009433925099E-5</c:v>
+                  <c:v>6.6032973700202993E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.2733400631695904E-5</c:v>
+                  <c:v>9.1826239950023594E-5</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>2.0665838383138101E-4</c:v>
+                  <c:v>1.8501331971492599E-4</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>4.36891580466181E-4</c:v>
+                  <c:v>4.3670004000887202E-4</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>1.07114161364734E-3</c:v>
+                  <c:v>1.07894792687147E-3</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>2.4844876141287301E-3</c:v>
+                  <c:v>2.6988179399631898E-3</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>5.9574958169832798E-3</c:v>
+                  <c:v>6.34287457796745E-3</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
-                  <c:v>1.4177412388380601E-2</c:v>
+                  <c:v>1.5447837053216E-2</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>3.40078002074733E-2</c:v>
+                  <c:v>3.4396914600511003E-2</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>7.7598812500946204E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.178692003979813</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.41521392923314099</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.98155113327084098</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.2970354792894701</c:v>
+                  <c:v>7.9342790392693097E-2</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>0.18683972923376099</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>0.43679219301848199</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>1.04754431002773</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>2.6486301862337802</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>5.6326177082140898</c:v>
+                  <c:v>6.5284631966572402</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>14.5183411833015</c:v>
+                  <c:v>16.096170290021099</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
-                  <c:v>34.6804867958882</c:v>
+                  <c:v>37.426206192138402</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1416,313 +1227,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000009-3C35-CA42-A871-90C9AD6AD040}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Exhaustive Search</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-3C35-CA42-A871-90C9AD6AD040}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000D-3C35-CA42-A871-90C9AD6AD040}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000F-3C35-CA42-A871-90C9AD6AD040}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000011-3C35-CA42-A871-90C9AD6AD040}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000013-3C35-CA42-A871-90C9AD6AD040}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000015-3C35-CA42-A871-90C9AD6AD040}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000017-3C35-CA42-A871-90C9AD6AD040}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="10"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000019-3C35-CA42-A871-90C9AD6AD040}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$1:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$1:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>2.4425087030977E-5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.9650092367082802E-5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0141825340688202E-5</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>1.93704187404364E-4</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>9.3917112099006696E-4</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>5.4293875000439498E-3</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>4.2910470569040599E-2</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>0.39486829169327298</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>4.1375219418900002</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>47.450318979192502</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000001A-3C35-CA42-A871-90C9AD6AD040}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2175,7 +1679,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$1:$P$19</c:f>
+              <c:f>Sheet1!$P$2:$P$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -2241,7 +1745,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$1:$Q$19</c:f>
+              <c:f>Sheet1!$R$2:$R$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -2249,58 +1753,58 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.7547636213822205E-3</c:v>
+                  <c:v>4.8530388581408797E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11120465886770201</c:v>
+                  <c:v>7.4340060101930894E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.1447315516620197E-2</c:v>
+                  <c:v>0.14624719087235499</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.19294272728707301</c:v>
+                  <c:v>0.149566194619697</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.29097037845258999</c:v>
+                  <c:v>0.24176598563923599</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.23838381521868099</c:v>
+                  <c:v>0.286223001233401</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16805656274129399</c:v>
+                  <c:v>0.24476540009601999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.241531244396512</c:v>
+                  <c:v>0.28067158644319001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.32319796638296799</c:v>
+                  <c:v>0.31877787709885802</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.41802707282386098</c:v>
+                  <c:v>0.35037577169596101</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.49681190055549701</c:v>
+                  <c:v>0.37680027236244801</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.25790531736163802</c:v>
+                  <c:v>0.37751646315566401</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.52394912681846395</c:v>
+                  <c:v>0.36468891721290803</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.40207687419960703</c:v>
+                  <c:v>0.37199854173965902</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.44725137509171597</c:v>
+                  <c:v>0.466522251482129</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.36569806706369301</c:v>
+                  <c:v>0.38173864782863998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.55610751928873203</c:v>
+                  <c:v>0.46126749725573901</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.48313867179154701</c:v>
+                  <c:v>0.45764996253545198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2328,7 +1832,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="square"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
@@ -2358,7 +1862,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$21:$P$39</c:f>
+              <c:f>Sheet1!$P$23:$P$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -2424,7 +1928,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$21:$Q$39</c:f>
+              <c:f>Sheet1!$R$23:$R$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -2432,58 +1936,58 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.46859859570989E-2</c:v>
+                  <c:v>6.3424028790807399E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.12784577092020599</c:v>
+                  <c:v>0.10538182688089601</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.4737496453859996E-2</c:v>
+                  <c:v>0.21658389708338999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32674613306043598</c:v>
+                  <c:v>0.26679899076942798</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.46385142500648102</c:v>
+                  <c:v>0.36194666270759501</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45840009580017499</c:v>
+                  <c:v>0.435025059056246</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.39300478933520799</c:v>
+                  <c:v>0.44287034170792899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.53164546037542904</c:v>
+                  <c:v>0.484358270517733</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.56850373763724005</c:v>
+                  <c:v>0.61463785979287899</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.79700874174263503</c:v>
+                  <c:v>0.76492082434018505</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.72914191469802803</c:v>
+                  <c:v>0.836566836096721</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.655277893981982</c:v>
+                  <c:v>0.88213386708022201</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0462722633155701</c:v>
+                  <c:v>0.94427919000523397</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.81460755007185703</c:v>
+                  <c:v>0.97507248608862596</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.92613724590865998</c:v>
+                  <c:v>1.11772021165422</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.1675024965740799</c:v>
+                  <c:v>1.05861191228193</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.34038524510091</c:v>
+                  <c:v>1.1015995826010001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.2346367360332</c:v>
+                  <c:v>1.2126892996032701</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2914,10 +2418,10 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Dynamic Programming</c:v>
+            <c:v>Greedy</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2943,81 +2447,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dPt>
-            <c:idx val="12"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000000-414D-594E-8F18-81DB34697FEC}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="13"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-414D-594E-8F18-81DB34697FEC}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="14"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000002-414D-594E-8F18-81DB34697FEC}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$13:$A$31</c:f>
+              <c:f>Sheet1!$P$2:$P$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -3083,66 +2515,66 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$B$31</c:f>
+              <c:f>Sheet1!$Q$2:$Q$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>3.2562599517405003E-5</c:v>
+                  <c:v>3.1999152852222297E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5354180727154E-5</c:v>
+                  <c:v>4.5802889508195202E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0225009433925099E-5</c:v>
+                  <c:v>2.5398246361873999E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.2733400631695904E-5</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>2.0665838383138101E-4</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>4.36891580466181E-4</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>1.07114161364734E-3</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>2.4844876141287301E-3</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>5.9574958169832798E-3</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>1.4177412388380601E-2</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>3.40078002074733E-2</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>7.7598812500946204E-2</c:v>
+                  <c:v>3.6299587809480702E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4229207667522102E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.1895820437930499E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4942040587775399E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.9032500246539702E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.4230457753874303E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.2327050836756803E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.8622928811237199E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.0749201481230498E-5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.178692003979813</c:v>
+                  <c:v>8.5122868767939494E-5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.41521392923314099</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.98155113327084098</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.2970354792894701</c:v>
+                  <c:v>9.6262507722713001E-5</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>1.02887448738329E-4</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>1.15071268519386E-4</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>5.6326177082140898</c:v>
+                  <c:v>1.2648907897528199E-4</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>14.5183411833015</c:v>
+                  <c:v>1.4632290112785899E-4</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
-                  <c:v>34.6804867958882</c:v>
+                  <c:v>1.5017792931757801E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3150,15 +2582,15 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-414D-594E-8F18-81DB34697FEC}"/>
+              <c16:uniqueId val="{0000000B-414D-594E-8F18-81DB34697FEC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Greedy</c:v>
+            <c:v>Minimum spanning tree</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -3170,7 +2602,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="square"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
@@ -3186,7 +2618,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$1:$P$19</c:f>
+              <c:f>Sheet1!$P$23:$P$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -3252,66 +2684,66 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$S$1:$S$19</c:f>
+              <c:f>Sheet1!$Q$23:$Q$41</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>3.5825002123601699E-5</c:v>
+                  <c:v>3.2971299951895997E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.4354098897892903E-5</c:v>
+                  <c:v>3.3389533637091501E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.17083991831168E-5</c:v>
+                  <c:v>2.9686250491067701E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6779201764147702E-5</c:v>
+                  <c:v>3.7753392243757801E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9858299714978703E-5</c:v>
+                  <c:v>3.87733383104205E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.6095800644252399E-5</c:v>
+                  <c:v>5.5876628030091499E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.22289978107437E-5</c:v>
+                  <c:v>5.5494120460934902E-5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.7079103135038101E-5</c:v>
+                  <c:v>5.8279542136005998E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.8720702226273702E-5</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>1.0771249944809801E-4</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>1.4403740351554001E-4</c:v>
+                  <c:v>6.5972031443379799E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.6597078004851898E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.6431660456582897E-5</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>1.5826250164536701E-4</c:v>
+                  <c:v>1.05492080911062E-4</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>1.67962297564372E-4</c:v>
+                  <c:v>1.08628821326419E-4</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>1.8422069842927101E-4</c:v>
+                  <c:v>1.18197491974569E-4</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>1.91808499221224E-4</c:v>
+                  <c:v>1.34140453883446E-4</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>2.1978720033075599E-4</c:v>
+                  <c:v>1.4656541810836599E-4</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>2.2655820066574901E-4</c:v>
+                  <c:v>1.6175374854356E-4</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>3.6107909982092598E-4</c:v>
+                  <c:v>1.89826709101907E-4</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
-                  <c:v>9.8596230236580595E-4</c:v>
+                  <c:v>1.96829203050583E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3319,35 +2751,35 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-414D-594E-8F18-81DB34697FEC}"/>
+              <c16:uniqueId val="{0000000C-414D-594E-8F18-81DB34697FEC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Minimum spanning tree</c:v>
+            <c:v>Dynamic Programming</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="triangle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent3"/>
+                  <a:schemeClr val="accent6"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -3355,7 +2787,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$21:$P$39</c:f>
+              <c:f>Sheet1!$A$14:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -3421,66 +2853,66 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$S$21:$S$39</c:f>
+              <c:f>Sheet1!$B$14:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>4.6187700354494102E-5</c:v>
+                  <c:v>3.8732078974135202E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.3058401681482698E-5</c:v>
+                  <c:v>3.9045728626661003E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.4366501970216602E-5</c:v>
+                  <c:v>6.6032973700202993E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8300101479981097E-5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.4966602076310602E-5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0300201585050602E-5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.4704300893936295E-5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6.80832003126852E-5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.2270900020375796E-5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.1658398266881696E-5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.3754001136403496E-5</c:v>
+                  <c:v>9.1826239950023594E-5</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>1.8501331971492599E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>4.3670004000887202E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>1.07894792687147E-3</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>2.6988179399631898E-3</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>6.34287457796745E-3</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>1.5447837053216E-2</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>3.4396914600511003E-2</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>1.06099997356068E-4</c:v>
+                  <c:v>7.9342790392693097E-2</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>1.1902499827556299E-4</c:v>
+                  <c:v>0.18683972923376099</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>1.3036659802310099E-4</c:v>
+                  <c:v>0.43679219301848199</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>1.47987499076407E-4</c:v>
+                  <c:v>1.04754431002773</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>1.6299589915433899E-4</c:v>
+                  <c:v>2.6486301862337802</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>1.7460410308558401E-4</c:v>
+                  <c:v>6.5284631966572402</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>1.90300005488097E-4</c:v>
+                  <c:v>16.096170290021099</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
-                  <c:v>2.1869589836569499E-4</c:v>
+                  <c:v>37.426206192138402</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3488,7 +2920,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-414D-594E-8F18-81DB34697FEC}"/>
+              <c16:uniqueId val="{00000003-414D-594E-8F18-81DB34697FEC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6201,30 +5633,22 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_br_2" connectionId="2" xr16:uid="{2968DE33-C909-9B4F-9608-A1CC59D8E9A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_dp_4" connectionId="3" xr16:uid="{C879CB0A-886A-1C42-8B97-490E43705B26}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_greedy" connectionId="6" xr16:uid="{659024B7-2775-A846-A03E-4C6233E34636}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_br_3" connectionId="2" xr16:uid="{E6DF8E23-2D7B-6F47-A9D0-12F9F6301448}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_mst" connectionId="7" xr16:uid="{D6160FED-F641-B34B-BFBC-438099521667}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_mst_1" connectionId="5" xr16:uid="{0CC94A00-BA83-9D44-A052-9898D8B654A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_dp" connectionId="3" xr16:uid="{A38A6EA9-0153-0D4A-9803-DC447E61790C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_greedy_1" connectionId="4" xr16:uid="{AB8857DE-6E74-2242-B4E3-FACC240DD61D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_dp_3" connectionId="4" xr16:uid="{431A5A0A-0D00-6746-A729-0C8671FDF2E8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_dp_2" connectionId="5" xr16:uid="{448F1A0E-9594-1D47-ADA1-8FA9959D8C52}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_br" connectionId="1" xr16:uid="{D13C840A-1D9F-8547-9FCE-E9EBA5D372AF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -6525,622 +5949,653 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB42E8F-E18A-D64A-A94C-602C99A3A6CC}">
-  <dimension ref="A1:W40"/>
+  <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C24" zoomScale="75" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="O57" sqref="O57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9" customWidth="1"/>
-    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2.4425087030977E-5</v>
-      </c>
-      <c r="P1">
-        <v>3</v>
-      </c>
-      <c r="Q1">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="1">
-        <v>3.5825002123601699E-5</v>
-      </c>
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>3.9650092367082802E-5</v>
+        <v>3.2020428334362799E-5</v>
       </c>
       <c r="P2">
-        <v>4</v>
-      </c>
-      <c r="Q2">
-        <v>8.7547636213822205E-3</v>
-      </c>
-      <c r="S2" s="1">
-        <v>3.4354098897892903E-5</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>3.1999152852222297E-5</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>5.0141825340688202E-5</v>
+        <v>3.2641708385199303E-5</v>
       </c>
       <c r="P3">
-        <v>5</v>
-      </c>
-      <c r="Q3">
-        <v>0.11120465886770201</v>
-      </c>
-      <c r="S3" s="1">
-        <v>3.17083991831168E-5</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>4.5802889508195202E-5</v>
+      </c>
+      <c r="R3">
+        <v>4.8530388581408797E-2</v>
+      </c>
+      <c r="S3" s="1"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>1.93704187404364E-4</v>
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5.1525000017136302E-5</v>
       </c>
       <c r="P4">
-        <v>6</v>
-      </c>
-      <c r="Q4">
-        <v>8.1447315516620197E-2</v>
-      </c>
-      <c r="S4" s="1">
-        <v>3.6779201764147702E-5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>2.5398246361873999E-5</v>
+      </c>
+      <c r="R4">
+        <v>7.4340060101930894E-2</v>
+      </c>
+      <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>9.3917112099006696E-4</v>
+        <v>1.6029003134462901E-4</v>
       </c>
       <c r="P5">
-        <v>7</v>
-      </c>
-      <c r="Q5">
-        <v>0.19294272728707301</v>
-      </c>
-      <c r="S5" s="1">
-        <v>3.9858299714978703E-5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>3.6299587809480702E-5</v>
+      </c>
+      <c r="R5">
+        <v>0.14624719087235499</v>
+      </c>
+      <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>5.4293875000439498E-3</v>
+        <v>8.0889039963949396E-4</v>
       </c>
       <c r="P6">
-        <v>8</v>
-      </c>
-      <c r="Q6">
-        <v>0.29097037845258999</v>
-      </c>
-      <c r="S6" s="1">
-        <v>4.6095800644252399E-5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>3.4229207667522102E-5</v>
+      </c>
+      <c r="R6">
+        <v>0.149566194619697</v>
+      </c>
+      <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>4.2910470569040599E-2</v>
+        <v>5.5364337802166104E-3</v>
       </c>
       <c r="P7">
-        <v>9</v>
-      </c>
-      <c r="Q7">
-        <v>0.23838381521868099</v>
-      </c>
-      <c r="S7" s="1">
-        <v>5.22289978107437E-5</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>7.1895820437930499E-5</v>
+      </c>
+      <c r="R7">
+        <v>0.24176598563923599</v>
+      </c>
+      <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>0.39486829169327298</v>
+        <v>4.4285878327791503E-2</v>
       </c>
       <c r="P8">
-        <v>10</v>
-      </c>
-      <c r="Q8">
-        <v>0.16805656274129399</v>
-      </c>
-      <c r="S8" s="1">
-        <v>5.7079103135038101E-5</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>5.4942040587775399E-5</v>
+      </c>
+      <c r="R8">
+        <v>0.286223001233401</v>
+      </c>
+      <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>4.1375219418900002</v>
+        <v>0.40938890543067802</v>
       </c>
       <c r="P9">
-        <v>11</v>
-      </c>
-      <c r="Q9">
-        <v>0.241531244396512</v>
-      </c>
-      <c r="S9" s="1">
-        <v>9.8720702226273702E-5</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>4.9032500246539702E-5</v>
+      </c>
+      <c r="R9">
+        <v>0.24476540009601999</v>
+      </c>
+      <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>47.450318979192502</v>
+        <v>4.4097970754495996</v>
       </c>
       <c r="P10">
-        <v>12</v>
-      </c>
-      <c r="Q10">
-        <v>0.32319796638296799</v>
-      </c>
-      <c r="S10">
-        <v>1.0771249944809801E-4</v>
+        <v>11</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>5.4230457753874303E-5</v>
+      </c>
+      <c r="R10">
+        <v>0.28067158644319001</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>52.464114895861101</v>
+      </c>
       <c r="P11">
-        <v>13</v>
-      </c>
-      <c r="Q11">
-        <v>0.41802707282386098</v>
-      </c>
-      <c r="S11">
-        <v>1.4403740351554001E-4</v>
+        <v>12</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>6.2327050836756803E-5</v>
+      </c>
+      <c r="R11">
+        <v>0.31877787709885802</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="P12">
-        <v>14</v>
-      </c>
-      <c r="Q12">
-        <v>0.49681190055549701</v>
-      </c>
-      <c r="S12">
-        <v>1.5826250164536701E-4</v>
+        <v>13</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>6.8622928811237199E-5</v>
+      </c>
+      <c r="R12">
+        <v>0.35037577169596101</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1">
-        <v>3.2562599517405003E-5</v>
-      </c>
       <c r="P13">
-        <v>15</v>
-      </c>
-      <c r="Q13">
-        <v>0.25790531736163802</v>
-      </c>
-      <c r="S13">
-        <v>1.67962297564372E-4</v>
+        <v>14</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>9.0749201481230498E-5</v>
+      </c>
+      <c r="R13">
+        <v>0.37680027236244801</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="1">
-        <v>3.5354180727154E-5</v>
+        <v>3.8732078974135202E-5</v>
       </c>
       <c r="P14">
-        <v>16</v>
-      </c>
-      <c r="Q14">
-        <v>0.52394912681846395</v>
-      </c>
-      <c r="S14">
-        <v>1.8422069842927101E-4</v>
+        <v>15</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>8.5122868767939494E-5</v>
+      </c>
+      <c r="R14">
+        <v>0.37751646315566401</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="1">
-        <v>4.0225009433925099E-5</v>
+        <v>3.9045728626661003E-5</v>
       </c>
       <c r="P15">
-        <v>17</v>
-      </c>
-      <c r="Q15">
-        <v>0.40207687419960703</v>
-      </c>
-      <c r="S15">
-        <v>1.91808499221224E-4</v>
+        <v>16</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>9.6262507722713001E-5</v>
+      </c>
+      <c r="R15">
+        <v>0.36468891721290803</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="1">
-        <v>8.2733400631695904E-5</v>
+        <v>6.6032973700202993E-5</v>
       </c>
       <c r="P16">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q16">
-        <v>0.44725137509171597</v>
-      </c>
-      <c r="S16">
-        <v>2.1978720033075599E-4</v>
+        <v>1.02887448738329E-4</v>
+      </c>
+      <c r="R16">
+        <v>0.37199854173965902</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>7</v>
-      </c>
-      <c r="B17">
-        <v>2.0665838383138101E-4</v>
+        <v>6</v>
+      </c>
+      <c r="B17" s="1">
+        <v>9.1826239950023594E-5</v>
       </c>
       <c r="P17">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q17">
-        <v>0.36569806706369301</v>
-      </c>
-      <c r="S17">
-        <v>2.2655820066574901E-4</v>
+        <v>1.15071268519386E-4</v>
+      </c>
+      <c r="R17">
+        <v>0.466522251482129</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18">
-        <v>4.36891580466181E-4</v>
+        <v>1.8501331971492599E-4</v>
       </c>
       <c r="P18">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q18">
-        <v>0.55610751928873203</v>
-      </c>
-      <c r="S18">
-        <v>3.6107909982092598E-4</v>
+        <v>1.2648907897528199E-4</v>
+      </c>
+      <c r="R18">
+        <v>0.38173864782863998</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19">
-        <v>1.07114161364734E-3</v>
+        <v>4.3670004000887202E-4</v>
       </c>
       <c r="P19">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q19">
-        <v>0.48313867179154701</v>
-      </c>
-      <c r="S19">
-        <v>9.8596230236580595E-4</v>
+        <v>1.4632290112785899E-4</v>
+      </c>
+      <c r="R19">
+        <v>0.46126749725573901</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20">
-        <v>2.4844876141287301E-3</v>
+        <v>1.07894792687147E-3</v>
+      </c>
+      <c r="P20">
+        <v>21</v>
+      </c>
+      <c r="Q20">
+        <v>1.5017792931757801E-4</v>
+      </c>
+      <c r="R20">
+        <v>0.45764996253545198</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21">
-        <v>5.9574958169832798E-3</v>
-      </c>
-      <c r="P21">
-        <v>3</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="S21" s="1">
-        <v>4.6187700354494102E-5</v>
+        <v>2.6988179399631898E-3</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22">
-        <v>1.4177412388380601E-2</v>
-      </c>
-      <c r="P22">
-        <v>4</v>
-      </c>
-      <c r="Q22">
-        <v>5.46859859570989E-2</v>
-      </c>
-      <c r="S22" s="1">
-        <v>5.3058401681482698E-5</v>
-      </c>
+        <v>6.34287457796745E-3</v>
+      </c>
+      <c r="S22" s="1"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B23">
-        <v>3.40078002074733E-2</v>
+        <v>1.5447837053216E-2</v>
       </c>
       <c r="P23">
-        <v>5</v>
-      </c>
-      <c r="Q23">
-        <v>0.12784577092020599</v>
-      </c>
-      <c r="S23" s="1">
-        <v>4.4366501970216602E-5</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>3.2971299951895997E-5</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24">
-        <v>7.7598812500946204E-2</v>
+        <v>3.4396914600511003E-2</v>
       </c>
       <c r="P24">
-        <v>6</v>
-      </c>
-      <c r="Q24">
-        <v>9.4737496453859996E-2</v>
-      </c>
-      <c r="S24" s="1">
-        <v>4.8300101479981097E-5</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>3.3389533637091501E-5</v>
+      </c>
+      <c r="R24">
+        <v>6.3424028790807399E-2</v>
+      </c>
+      <c r="S24" s="1"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>15</v>
-      </c>
-      <c r="B25" s="1">
-        <v>0.178692003979813</v>
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>7.9342790392693097E-2</v>
       </c>
       <c r="P25">
-        <v>7</v>
-      </c>
-      <c r="Q25">
-        <v>0.32674613306043598</v>
-      </c>
-      <c r="S25" s="1">
-        <v>6.4966602076310602E-5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>2.9686250491067701E-5</v>
+      </c>
+      <c r="R25">
+        <v>0.10538182688089601</v>
+      </c>
+      <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>16</v>
-      </c>
-      <c r="B26" s="1">
-        <v>0.41521392923314099</v>
+        <v>15</v>
+      </c>
+      <c r="B26">
+        <v>0.18683972923376099</v>
       </c>
       <c r="P26">
-        <v>8</v>
-      </c>
-      <c r="Q26">
-        <v>0.46385142500648102</v>
-      </c>
-      <c r="S26" s="1">
-        <v>6.0300201585050602E-5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>3.7753392243757801E-5</v>
+      </c>
+      <c r="R26">
+        <v>0.21658389708338999</v>
+      </c>
+      <c r="S26" s="1"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>17</v>
-      </c>
-      <c r="B27" s="1">
-        <v>0.98155113327084098</v>
+        <v>16</v>
+      </c>
+      <c r="B27">
+        <v>0.43679219301848199</v>
       </c>
       <c r="P27">
-        <v>9</v>
-      </c>
-      <c r="Q27">
-        <v>0.45840009580017499</v>
-      </c>
-      <c r="S27" s="1">
-        <v>6.4704300893936295E-5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>3.87733383104205E-5</v>
+      </c>
+      <c r="R27">
+        <v>0.26679899076942798</v>
+      </c>
+      <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>18</v>
-      </c>
-      <c r="B28" s="1">
-        <v>2.2970354792894701</v>
+        <v>17</v>
+      </c>
+      <c r="B28">
+        <v>1.04754431002773</v>
       </c>
       <c r="P28">
-        <v>10</v>
-      </c>
-      <c r="Q28">
-        <v>0.39300478933520799</v>
-      </c>
-      <c r="S28" s="1">
-        <v>6.80832003126852E-5</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>5.5876628030091499E-5</v>
+      </c>
+      <c r="R28">
+        <v>0.36194666270759501</v>
+      </c>
+      <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29">
-        <v>5.6326177082140898</v>
+        <v>2.6486301862337802</v>
       </c>
       <c r="P29">
-        <v>11</v>
-      </c>
-      <c r="Q29">
-        <v>0.53164546037542904</v>
-      </c>
-      <c r="S29" s="1">
-        <v>8.2270900020375796E-5</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>5.5494120460934902E-5</v>
+      </c>
+      <c r="R29">
+        <v>0.435025059056246</v>
+      </c>
+      <c r="S29" s="1"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B30">
-        <v>14.5183411833015</v>
+        <v>6.5284631966572402</v>
       </c>
       <c r="P30">
-        <v>12</v>
-      </c>
-      <c r="Q30">
-        <v>0.56850373763724005</v>
-      </c>
-      <c r="S30" s="1">
-        <v>8.1658398266881696E-5</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>5.8279542136005998E-5</v>
+      </c>
+      <c r="R30">
+        <v>0.44287034170792899</v>
+      </c>
+      <c r="S30" s="1"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31">
-        <v>34.6804867958882</v>
+        <v>16.096170290021099</v>
       </c>
       <c r="P31">
-        <v>13</v>
-      </c>
-      <c r="Q31">
-        <v>0.79700874174263503</v>
-      </c>
-      <c r="S31" s="1">
-        <v>9.3754001136403496E-5</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>6.5972031443379799E-5</v>
+      </c>
+      <c r="R31">
+        <v>0.484358270517733</v>
+      </c>
+      <c r="S31" s="1"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>21</v>
+      </c>
+      <c r="B32">
+        <v>37.426206192138402</v>
+      </c>
       <c r="P32">
-        <v>14</v>
-      </c>
-      <c r="Q32">
-        <v>0.72914191469802803</v>
-      </c>
-      <c r="S32">
-        <v>1.06099997356068E-4</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>7.6597078004851898E-5</v>
+      </c>
+      <c r="R32">
+        <v>0.61463785979287899</v>
+      </c>
+      <c r="S32" s="1"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.2">
       <c r="P33">
-        <v>15</v>
-      </c>
-      <c r="Q33">
-        <v>0.655277893981982</v>
-      </c>
-      <c r="S33">
-        <v>1.1902499827556299E-4</v>
+        <v>13</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>8.6431660456582897E-5</v>
+      </c>
+      <c r="R33">
+        <v>0.76492082434018505</v>
       </c>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.2">
       <c r="P34">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Q34">
-        <v>1.0462722633155701</v>
-      </c>
-      <c r="S34">
-        <v>1.3036659802310099E-4</v>
+        <v>1.05492080911062E-4</v>
+      </c>
+      <c r="R34">
+        <v>0.836566836096721</v>
       </c>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.2">
       <c r="P35">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q35">
-        <v>0.81460755007185703</v>
-      </c>
-      <c r="S35">
-        <v>1.47987499076407E-4</v>
+        <v>1.08628821326419E-4</v>
+      </c>
+      <c r="R35">
+        <v>0.88213386708022201</v>
       </c>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.2">
       <c r="P36">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Q36">
-        <v>0.92613724590865998</v>
-      </c>
-      <c r="S36">
-        <v>1.6299589915433899E-4</v>
+        <v>1.18197491974569E-4</v>
+      </c>
+      <c r="R36">
+        <v>0.94427919000523397</v>
       </c>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.2">
       <c r="P37">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q37">
-        <v>1.1675024965740799</v>
-      </c>
-      <c r="S37">
-        <v>1.7460410308558401E-4</v>
+        <v>1.34140453883446E-4</v>
+      </c>
+      <c r="R37">
+        <v>0.97507248608862596</v>
       </c>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B38" s="1"/>
       <c r="P38">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Q38">
-        <v>1.34038524510091</v>
-      </c>
-      <c r="S38">
-        <v>1.90300005488097E-4</v>
+        <v>1.4656541810836599E-4</v>
+      </c>
+      <c r="R38">
+        <v>1.11772021165422</v>
       </c>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B39" s="1"/>
       <c r="P39">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q39">
-        <v>1.2346367360332</v>
-      </c>
-      <c r="S39">
-        <v>2.1869589836569499E-4</v>
+        <v>1.6175374854356E-4</v>
+      </c>
+      <c r="R39">
+        <v>1.05861191228193</v>
       </c>
       <c r="W39" s="2"/>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B40" s="1"/>
+      <c r="P40">
+        <v>20</v>
+      </c>
+      <c r="Q40">
+        <v>1.89826709101907E-4</v>
+      </c>
+      <c r="R40">
+        <v>1.1015995826010001</v>
+      </c>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="P41">
+        <v>21</v>
+      </c>
+      <c r="Q41">
+        <v>1.96829203050583E-4</v>
+      </c>
+      <c r="R41">
+        <v>1.2126892996032701</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add more data to heuristic benchmark
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933FA35E-2C52-4744-9BB4-2A391CAD9EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CA0330-0DAD-1F4F-A3FF-9578F286F06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4940" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{75212AE2-A3F9-034E-9D2E-443F9B0F6379}"/>
   </bookViews>
@@ -23,7 +23,9 @@
     <definedName name="result_dp_2" localSheetId="0">Sheet1!#REF!</definedName>
     <definedName name="result_dp_3" localSheetId="0">Sheet1!#REF!</definedName>
     <definedName name="result_dp_4" localSheetId="0">Sheet1!$A$14:$B$32</definedName>
+    <definedName name="result_greedy" localSheetId="0">Sheet1!$AH$44:$AI$140</definedName>
     <definedName name="result_greedy_1" localSheetId="0">Sheet1!$P$2:$R$81</definedName>
+    <definedName name="result_mst" localSheetId="0">Sheet1!$AK$17:$AM$94</definedName>
     <definedName name="result_mst_1" localSheetId="0">Sheet1!$AF$5:$AH$43</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -56,7 +58,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{31346737-7074-834E-ADE2-73C90860B480}" name="result_br1" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" firstRow="24" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_br.txt" tab="0" space="1" consecutive="1">
+    <textPr firstRow="24" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_br.txt" tab="0" space="1" consecutive="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -68,7 +70,7 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{46BFB1C6-60FC-E246-856D-4A76B7E1C519}" name="result_dp3" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" firstRow="24" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_dp.txt" tab="0" space="1" consecutive="1">
+    <textPr firstRow="24" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_dp.txt" tab="0" space="1" consecutive="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -79,8 +81,18 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{E574AEC5-39E1-7045-BDA9-CB3CD0FBC749}" name="result_greedy1" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" firstRow="23" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_greedy.txt" tab="0" space="1" consecutive="1">
+  <connection id="4" xr16:uid="{1F537394-A657-2146-BBE2-43BB3C8A7AF5}" name="result_greedy" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" firstRow="46" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_greedy.txt" tab="0" space="1" consecutive="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" xr16:uid="{E574AEC5-39E1-7045-BDA9-CB3CD0FBC749}" name="result_greedy1" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="23" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_greedy.txt" tab="0" space="1" consecutive="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -88,8 +100,17 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" xr16:uid="{DC51D5A7-BA3B-3A49-8F6D-60E3001D7191}" name="result_mst1" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" firstRow="23" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_mst.txt" tab="0" space="1" consecutive="1">
+  <connection id="6" xr16:uid="{FAA8EE6E-ED42-1846-B150-AED62FE4385A}" name="result_mst" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" firstRow="65" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_mst.txt" tab="0" space="1" consecutive="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" xr16:uid="{DC51D5A7-BA3B-3A49-8F6D-60E3001D7191}" name="result_mst1" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr firstRow="23" sourceFile="/Users/quocmai/Uni/COS10009/Portfolio/HD10.4/result_mst.txt" tab="0" space="1" consecutive="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -101,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>runtime</t>
   </si>
@@ -1862,7 +1883,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$23:$P$41</c:f>
+              <c:f>Sheet1!$T$2:$T$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1928,7 +1949,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$23:$R$41</c:f>
+              <c:f>Sheet1!$V$2:$V$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -2449,10 +2470,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$20</c:f>
+              <c:f>Sheet1!$P$2:$P$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -2509,16 +2530,103 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$20</c:f>
+              <c:f>Sheet1!$Q$2:$Q$49</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>3.1999152852222297E-5</c:v>
                 </c:pt>
@@ -2575,6 +2683,93 @@
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
                   <c:v>1.5017792931757801E-4</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>2.42440861766226E-4</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>2.2155917948111801E-4</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>2.4505336012225598E-4</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>2.9299041081685501E-4</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>2.9253505461383599E-4</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>3.1717457983177101E-4</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="General">
+                  <c:v>3.05666667409241E-4</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="General">
+                  <c:v>4.0294378472026398E-4</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="General">
+                  <c:v>3.8863842200953503E-4</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="General">
+                  <c:v>4.0731753106228999E-4</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="General">
+                  <c:v>4.1791173280216701E-4</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="General">
+                  <c:v>5.1787584729026995E-4</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="General">
+                  <c:v>4.3275714910123399E-4</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="General">
+                  <c:v>4.6448578126728502E-4</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="General">
+                  <c:v>5.1110086031258095E-4</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="General">
+                  <c:v>4.86731767305172E-4</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="General">
+                  <c:v>5.6325701938476404E-4</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="General">
+                  <c:v>5.8113002975005595E-4</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="General">
+                  <c:v>5.5167663027532398E-4</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="General">
+                  <c:v>5.8261668833438298E-4</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="General">
+                  <c:v>6.2285214022267605E-4</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="General">
+                  <c:v>6.6502464469522197E-4</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="General">
+                  <c:v>6.6327872278634402E-4</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="General">
+                  <c:v>7.0417544222436805E-4</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="General">
+                  <c:v>7.4928707210346996E-4</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="General">
+                  <c:v>7.9405041062272997E-4</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="General">
+                  <c:v>8.2994122116360799E-4</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="General">
+                  <c:v>8.3986910933163004E-4</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>8.6233335721772096E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2618,10 +2813,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$23:$P$41</c:f>
+              <c:f>Sheet1!$T$2:$T$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -2678,16 +2873,103 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$23:$Q$41</c:f>
+              <c:f>Sheet1!$U$2:$U$49</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>3.2971299951895997E-5</c:v>
                 </c:pt>
@@ -2744,6 +3026,93 @@
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
                   <c:v>1.96829203050583E-4</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>3.06918732239864E-4</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>3.3350291196256802E-4</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>3.34684172994457E-4</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>4.1422798996791198E-4</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>4.0173461020458402E-4</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>4.1275335301179397E-4</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="General">
+                  <c:v>4.1027205181308002E-4</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="General">
+                  <c:v>4.7916959447320498E-4</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="General">
+                  <c:v>5.3328707756008901E-4</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="General">
+                  <c:v>5.5316461890470199E-4</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="General">
+                  <c:v>5.3784997202455998E-4</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="General">
+                  <c:v>7.2794711100868797E-4</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="General">
+                  <c:v>5.7775584922637705E-4</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="General">
+                  <c:v>6.3408672111108899E-4</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="General">
+                  <c:v>6.75467522814869E-4</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="General">
+                  <c:v>6.8319666024763105E-4</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="General">
+                  <c:v>7.9426876036450204E-4</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="General">
+                  <c:v>7.9887119005434199E-4</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="General">
+                  <c:v>7.5030748092103701E-4</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="General">
+                  <c:v>7.9575834912247901E-4</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="General">
+                  <c:v>8.8708043680526302E-4</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="General">
+                  <c:v>9.6447086776606705E-4</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="General">
+                  <c:v>9.34135454008355E-4</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="General">
+                  <c:v>9.8733918275684097E-4</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="General">
+                  <c:v>1.0395349666941899E-3</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="General">
+                  <c:v>1.1197758233174599E-3</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="General">
+                  <c:v>1.1817599966889201E-3</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="General">
+                  <c:v>1.1917682777857401E-3</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>1.2285449868068099E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5555,16 +5924,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>524933</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>182804</xdr:rowOff>
+      <xdr:rowOff>199737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>221287</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>255154</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>35682</xdr:rowOff>
+      <xdr:rowOff>52615</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5593,16 +5962,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>89648</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>430449</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>124581</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>360149</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5633,22 +6002,30 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_mst" connectionId="6" xr16:uid="{401BC3CE-6A3C-DA4E-8660-21EEC60DCAB2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_greedy" connectionId="4" xr16:uid="{3FFAB303-AFC7-FB4E-9BE1-8384E7F88972}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_dp_4" connectionId="3" xr16:uid="{C879CB0A-886A-1C42-8B97-490E43705B26}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_br_3" connectionId="2" xr16:uid="{E6DF8E23-2D7B-6F47-A9D0-12F9F6301448}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_mst_1" connectionId="5" xr16:uid="{0CC94A00-BA83-9D44-A052-9898D8B654A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_mst_1" connectionId="7" xr16:uid="{0CC94A00-BA83-9D44-A052-9898D8B654A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_greedy_1" connectionId="4" xr16:uid="{AB8857DE-6E74-2242-B4E3-FACC240DD61D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_greedy_1" connectionId="5" xr16:uid="{AB8857DE-6E74-2242-B4E3-FACC240DD61D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_br" connectionId="1" xr16:uid="{D13C840A-1D9F-8547-9FCE-E9EBA5D372AF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -5949,10 +6326,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB42E8F-E18A-D64A-A94C-602C99A3A6CC}">
-  <dimension ref="A1:W41"/>
+  <dimension ref="A1:W98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="O57" sqref="O57"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="67" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AG34" sqref="AG34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5964,11 +6341,17 @@
     <col min="16" max="16" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.6640625" customWidth="1"/>
     <col min="32" max="32" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.6640625" customWidth="1"/>
+    <col min="35" max="35" width="17.5" customWidth="1"/>
+    <col min="37" max="37" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="2.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -5979,8 +6362,14 @@
         <v>1</v>
       </c>
       <c r="S1" s="1"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -5997,8 +6386,17 @@
         <v>0</v>
       </c>
       <c r="S2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T2">
+        <v>3</v>
+      </c>
+      <c r="U2" s="1">
+        <v>3.2971299951895997E-5</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4</v>
       </c>
@@ -6015,8 +6413,17 @@
         <v>4.8530388581408797E-2</v>
       </c>
       <c r="S3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T3">
+        <v>4</v>
+      </c>
+      <c r="U3" s="1">
+        <v>3.3389533637091501E-5</v>
+      </c>
+      <c r="V3">
+        <v>6.3424028790807399E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5</v>
       </c>
@@ -6033,8 +6440,17 @@
         <v>7.4340060101930894E-2</v>
       </c>
       <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T4">
+        <v>5</v>
+      </c>
+      <c r="U4" s="1">
+        <v>2.9686250491067701E-5</v>
+      </c>
+      <c r="V4">
+        <v>0.10538182688089601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>6</v>
       </c>
@@ -6051,8 +6467,17 @@
         <v>0.14624719087235499</v>
       </c>
       <c r="S5" s="1"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T5">
+        <v>6</v>
+      </c>
+      <c r="U5" s="1">
+        <v>3.7753392243757801E-5</v>
+      </c>
+      <c r="V5">
+        <v>0.21658389708338999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>7</v>
       </c>
@@ -6069,8 +6494,17 @@
         <v>0.149566194619697</v>
       </c>
       <c r="S6" s="1"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T6">
+        <v>7</v>
+      </c>
+      <c r="U6" s="1">
+        <v>3.87733383104205E-5</v>
+      </c>
+      <c r="V6">
+        <v>0.26679899076942798</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>8</v>
       </c>
@@ -6087,8 +6521,17 @@
         <v>0.24176598563923599</v>
       </c>
       <c r="S7" s="1"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T7">
+        <v>8</v>
+      </c>
+      <c r="U7" s="1">
+        <v>5.5876628030091499E-5</v>
+      </c>
+      <c r="V7">
+        <v>0.36194666270759501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>9</v>
       </c>
@@ -6105,8 +6548,17 @@
         <v>0.286223001233401</v>
       </c>
       <c r="S8" s="1"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T8">
+        <v>9</v>
+      </c>
+      <c r="U8" s="1">
+        <v>5.5494120460934902E-5</v>
+      </c>
+      <c r="V8">
+        <v>0.435025059056246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>10</v>
       </c>
@@ -6123,8 +6575,17 @@
         <v>0.24476540009601999</v>
       </c>
       <c r="S9" s="1"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T9">
+        <v>10</v>
+      </c>
+      <c r="U9" s="1">
+        <v>5.8279542136005998E-5</v>
+      </c>
+      <c r="V9">
+        <v>0.44287034170792899</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>11</v>
       </c>
@@ -6140,8 +6601,17 @@
       <c r="R10">
         <v>0.28067158644319001</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T10">
+        <v>11</v>
+      </c>
+      <c r="U10" s="1">
+        <v>6.5972031443379799E-5</v>
+      </c>
+      <c r="V10">
+        <v>0.484358270517733</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>12</v>
       </c>
@@ -6157,8 +6627,17 @@
       <c r="R11">
         <v>0.31877787709885802</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T11">
+        <v>12</v>
+      </c>
+      <c r="U11" s="1">
+        <v>7.6597078004851898E-5</v>
+      </c>
+      <c r="V11">
+        <v>0.61463785979287899</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="P12">
         <v>13</v>
       </c>
@@ -6168,8 +6647,17 @@
       <c r="R12">
         <v>0.35037577169596101</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T12">
+        <v>13</v>
+      </c>
+      <c r="U12" s="1">
+        <v>8.6431660456582897E-5</v>
+      </c>
+      <c r="V12">
+        <v>0.76492082434018505</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="P13">
         <v>14</v>
       </c>
@@ -6179,8 +6667,17 @@
       <c r="R13">
         <v>0.37680027236244801</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T13">
+        <v>14</v>
+      </c>
+      <c r="U13">
+        <v>1.05492080911062E-4</v>
+      </c>
+      <c r="V13">
+        <v>0.836566836096721</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
@@ -6196,8 +6693,17 @@
       <c r="R14">
         <v>0.37751646315566401</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T14">
+        <v>15</v>
+      </c>
+      <c r="U14">
+        <v>1.08628821326419E-4</v>
+      </c>
+      <c r="V14">
+        <v>0.88213386708022201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>4</v>
       </c>
@@ -6213,8 +6719,17 @@
       <c r="R15">
         <v>0.36468891721290803</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T15">
+        <v>16</v>
+      </c>
+      <c r="U15">
+        <v>1.18197491974569E-4</v>
+      </c>
+      <c r="V15">
+        <v>0.94427919000523397</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
@@ -6230,8 +6745,17 @@
       <c r="R16">
         <v>0.37199854173965902</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T16">
+        <v>17</v>
+      </c>
+      <c r="U16">
+        <v>1.34140453883446E-4</v>
+      </c>
+      <c r="V16">
+        <v>0.97507248608862596</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -6247,8 +6771,17 @@
       <c r="R17">
         <v>0.466522251482129</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T17">
+        <v>18</v>
+      </c>
+      <c r="U17">
+        <v>1.4656541810836599E-4</v>
+      </c>
+      <c r="V17">
+        <v>1.11772021165422</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7</v>
       </c>
@@ -6264,8 +6797,17 @@
       <c r="R18">
         <v>0.38173864782863998</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T18">
+        <v>19</v>
+      </c>
+      <c r="U18">
+        <v>1.6175374854356E-4</v>
+      </c>
+      <c r="V18">
+        <v>1.05861191228193</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>8</v>
       </c>
@@ -6281,8 +6823,17 @@
       <c r="R19">
         <v>0.46126749725573901</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T19">
+        <v>20</v>
+      </c>
+      <c r="U19">
+        <v>1.89826709101907E-4</v>
+      </c>
+      <c r="V19">
+        <v>1.1015995826010001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>9</v>
       </c>
@@ -6298,25 +6849,58 @@
       <c r="R20">
         <v>0.45764996253545198</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T20">
+        <v>21</v>
+      </c>
+      <c r="U20">
+        <v>1.96829203050583E-4</v>
+      </c>
+      <c r="V20">
+        <v>1.2126892996032701</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>10</v>
       </c>
       <c r="B21">
         <v>2.6988179399631898E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="P21">
+        <v>22</v>
+      </c>
+      <c r="Q21">
+        <v>2.42440861766226E-4</v>
+      </c>
+      <c r="T21">
+        <v>22</v>
+      </c>
+      <c r="U21">
+        <v>3.06918732239864E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>11</v>
       </c>
       <c r="B22">
         <v>6.34287457796745E-3</v>
       </c>
+      <c r="P22">
+        <v>23</v>
+      </c>
+      <c r="Q22">
+        <v>2.2155917948111801E-4</v>
+      </c>
       <c r="S22" s="1"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T22">
+        <v>23</v>
+      </c>
+      <c r="U22">
+        <v>3.3350291196256802E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>12</v>
       </c>
@@ -6324,17 +6908,20 @@
         <v>1.5447837053216E-2</v>
       </c>
       <c r="P23">
-        <v>3</v>
-      </c>
-      <c r="Q23" s="1">
-        <v>3.2971299951895997E-5</v>
-      </c>
-      <c r="R23">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="Q23">
+        <v>2.4505336012225598E-4</v>
       </c>
       <c r="S23" s="1"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T23">
+        <v>24</v>
+      </c>
+      <c r="U23">
+        <v>3.34684172994457E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>13</v>
       </c>
@@ -6342,17 +6929,20 @@
         <v>3.4396914600511003E-2</v>
       </c>
       <c r="P24">
-        <v>4</v>
-      </c>
-      <c r="Q24" s="1">
-        <v>3.3389533637091501E-5</v>
-      </c>
-      <c r="R24">
-        <v>6.3424028790807399E-2</v>
+        <v>25</v>
+      </c>
+      <c r="Q24">
+        <v>2.9299041081685501E-4</v>
       </c>
       <c r="S24" s="1"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T24">
+        <v>25</v>
+      </c>
+      <c r="U24">
+        <v>4.1422798996791198E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>14</v>
       </c>
@@ -6360,17 +6950,20 @@
         <v>7.9342790392693097E-2</v>
       </c>
       <c r="P25">
-        <v>5</v>
-      </c>
-      <c r="Q25" s="1">
-        <v>2.9686250491067701E-5</v>
-      </c>
-      <c r="R25">
-        <v>0.10538182688089601</v>
+        <v>26</v>
+      </c>
+      <c r="Q25">
+        <v>2.9253505461383599E-4</v>
       </c>
       <c r="S25" s="1"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T25">
+        <v>26</v>
+      </c>
+      <c r="U25">
+        <v>4.0173461020458402E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>15</v>
       </c>
@@ -6378,17 +6971,20 @@
         <v>0.18683972923376099</v>
       </c>
       <c r="P26">
-        <v>6</v>
-      </c>
-      <c r="Q26" s="1">
-        <v>3.7753392243757801E-5</v>
-      </c>
-      <c r="R26">
-        <v>0.21658389708338999</v>
+        <v>27</v>
+      </c>
+      <c r="Q26">
+        <v>3.1717457983177101E-4</v>
       </c>
       <c r="S26" s="1"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T26">
+        <v>27</v>
+      </c>
+      <c r="U26">
+        <v>4.1275335301179397E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>16</v>
       </c>
@@ -6396,17 +6992,20 @@
         <v>0.43679219301848199</v>
       </c>
       <c r="P27">
-        <v>7</v>
-      </c>
-      <c r="Q27" s="1">
-        <v>3.87733383104205E-5</v>
-      </c>
-      <c r="R27">
-        <v>0.26679899076942798</v>
+        <v>28</v>
+      </c>
+      <c r="Q27">
+        <v>3.05666667409241E-4</v>
       </c>
       <c r="S27" s="1"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T27">
+        <v>28</v>
+      </c>
+      <c r="U27">
+        <v>4.1027205181308002E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>17</v>
       </c>
@@ -6414,17 +7013,20 @@
         <v>1.04754431002773</v>
       </c>
       <c r="P28">
-        <v>8</v>
-      </c>
-      <c r="Q28" s="1">
-        <v>5.5876628030091499E-5</v>
-      </c>
-      <c r="R28">
-        <v>0.36194666270759501</v>
+        <v>29</v>
+      </c>
+      <c r="Q28">
+        <v>4.0294378472026398E-4</v>
       </c>
       <c r="S28" s="1"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T28">
+        <v>29</v>
+      </c>
+      <c r="U28">
+        <v>4.7916959447320498E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>18</v>
       </c>
@@ -6432,17 +7034,20 @@
         <v>2.6486301862337802</v>
       </c>
       <c r="P29">
-        <v>9</v>
-      </c>
-      <c r="Q29" s="1">
-        <v>5.5494120460934902E-5</v>
-      </c>
-      <c r="R29">
-        <v>0.435025059056246</v>
+        <v>30</v>
+      </c>
+      <c r="Q29">
+        <v>3.8863842200953503E-4</v>
       </c>
       <c r="S29" s="1"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T29">
+        <v>30</v>
+      </c>
+      <c r="U29">
+        <v>5.3328707756008901E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>19</v>
       </c>
@@ -6450,17 +7055,20 @@
         <v>6.5284631966572402</v>
       </c>
       <c r="P30">
-        <v>10</v>
-      </c>
-      <c r="Q30" s="1">
-        <v>5.8279542136005998E-5</v>
-      </c>
-      <c r="R30">
-        <v>0.44287034170792899</v>
+        <v>31</v>
+      </c>
+      <c r="Q30">
+        <v>4.0731753106228999E-4</v>
       </c>
       <c r="S30" s="1"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T30">
+        <v>31</v>
+      </c>
+      <c r="U30">
+        <v>5.5316461890470199E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20</v>
       </c>
@@ -6468,17 +7076,20 @@
         <v>16.096170290021099</v>
       </c>
       <c r="P31">
-        <v>11</v>
-      </c>
-      <c r="Q31" s="1">
-        <v>6.5972031443379799E-5</v>
-      </c>
-      <c r="R31">
-        <v>0.484358270517733</v>
+        <v>32</v>
+      </c>
+      <c r="Q31">
+        <v>4.1791173280216701E-4</v>
       </c>
       <c r="S31" s="1"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T31">
+        <v>32</v>
+      </c>
+      <c r="U31">
+        <v>5.3784997202455998E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>21</v>
       </c>
@@ -6486,115 +7097,943 @@
         <v>37.426206192138402</v>
       </c>
       <c r="P32">
-        <v>12</v>
-      </c>
-      <c r="Q32" s="1">
-        <v>7.6597078004851898E-5</v>
-      </c>
-      <c r="R32">
-        <v>0.61463785979287899</v>
+        <v>33</v>
+      </c>
+      <c r="Q32">
+        <v>5.1787584729026995E-4</v>
       </c>
       <c r="S32" s="1"/>
+      <c r="T32">
+        <v>33</v>
+      </c>
+      <c r="U32">
+        <v>7.2794711100868797E-4</v>
+      </c>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.2">
       <c r="P33">
-        <v>13</v>
-      </c>
-      <c r="Q33" s="1">
-        <v>8.6431660456582897E-5</v>
-      </c>
-      <c r="R33">
-        <v>0.76492082434018505</v>
+        <v>34</v>
+      </c>
+      <c r="Q33">
+        <v>4.3275714910123399E-4</v>
+      </c>
+      <c r="T33">
+        <v>34</v>
+      </c>
+      <c r="U33">
+        <v>5.7775584922637705E-4</v>
       </c>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.2">
       <c r="P34">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="Q34">
-        <v>1.05492080911062E-4</v>
-      </c>
-      <c r="R34">
-        <v>0.836566836096721</v>
+        <v>4.6448578126728502E-4</v>
+      </c>
+      <c r="T34">
+        <v>35</v>
+      </c>
+      <c r="U34">
+        <v>6.3408672111108899E-4</v>
       </c>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.2">
       <c r="P35">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="Q35">
-        <v>1.08628821326419E-4</v>
-      </c>
-      <c r="R35">
-        <v>0.88213386708022201</v>
+        <v>5.1110086031258095E-4</v>
+      </c>
+      <c r="T35">
+        <v>36</v>
+      </c>
+      <c r="U35">
+        <v>6.75467522814869E-4</v>
       </c>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.2">
       <c r="P36">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="Q36">
-        <v>1.18197491974569E-4</v>
-      </c>
-      <c r="R36">
-        <v>0.94427919000523397</v>
+        <v>4.86731767305172E-4</v>
+      </c>
+      <c r="T36">
+        <v>37</v>
+      </c>
+      <c r="U36">
+        <v>6.8319666024763105E-4</v>
       </c>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.2">
       <c r="P37">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="Q37">
-        <v>1.34140453883446E-4</v>
-      </c>
-      <c r="R37">
-        <v>0.97507248608862596</v>
+        <v>5.6325701938476404E-4</v>
+      </c>
+      <c r="T37">
+        <v>38</v>
+      </c>
+      <c r="U37">
+        <v>7.9426876036450204E-4</v>
       </c>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B38" s="1"/>
       <c r="P38">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="Q38">
-        <v>1.4656541810836599E-4</v>
-      </c>
-      <c r="R38">
-        <v>1.11772021165422</v>
+        <v>5.8113002975005595E-4</v>
+      </c>
+      <c r="T38">
+        <v>39</v>
+      </c>
+      <c r="U38">
+        <v>7.9887119005434199E-4</v>
       </c>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.2">
       <c r="P39">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="Q39">
-        <v>1.6175374854356E-4</v>
-      </c>
-      <c r="R39">
-        <v>1.05861191228193</v>
+        <v>5.5167663027532398E-4</v>
+      </c>
+      <c r="T39">
+        <v>40</v>
+      </c>
+      <c r="U39">
+        <v>7.5030748092103701E-4</v>
       </c>
       <c r="W39" s="2"/>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.2">
       <c r="P40">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="Q40">
-        <v>1.89826709101907E-4</v>
-      </c>
-      <c r="R40">
-        <v>1.1015995826010001</v>
+        <v>5.8261668833438298E-4</v>
+      </c>
+      <c r="T40">
+        <v>41</v>
+      </c>
+      <c r="U40">
+        <v>7.9575834912247901E-4</v>
       </c>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.2">
       <c r="P41">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="Q41">
-        <v>1.96829203050583E-4</v>
-      </c>
-      <c r="R41">
-        <v>1.2126892996032701</v>
+        <v>6.2285214022267605E-4</v>
+      </c>
+      <c r="T41">
+        <v>42</v>
+      </c>
+      <c r="U41">
+        <v>8.8708043680526302E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="P42">
+        <v>43</v>
+      </c>
+      <c r="Q42">
+        <v>6.6502464469522197E-4</v>
+      </c>
+      <c r="T42">
+        <v>43</v>
+      </c>
+      <c r="U42">
+        <v>9.6447086776606705E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="P43">
+        <v>44</v>
+      </c>
+      <c r="Q43">
+        <v>6.6327872278634402E-4</v>
+      </c>
+      <c r="T43">
+        <v>44</v>
+      </c>
+      <c r="U43">
+        <v>9.34135454008355E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="P44">
+        <v>45</v>
+      </c>
+      <c r="Q44">
+        <v>7.0417544222436805E-4</v>
+      </c>
+      <c r="T44">
+        <v>45</v>
+      </c>
+      <c r="U44">
+        <v>9.8733918275684097E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="P45">
+        <v>46</v>
+      </c>
+      <c r="Q45">
+        <v>7.4928707210346996E-4</v>
+      </c>
+      <c r="T45">
+        <v>46</v>
+      </c>
+      <c r="U45">
+        <v>1.0395349666941899E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="P46">
+        <v>47</v>
+      </c>
+      <c r="Q46">
+        <v>7.9405041062272997E-4</v>
+      </c>
+      <c r="T46">
+        <v>47</v>
+      </c>
+      <c r="U46">
+        <v>1.1197758233174599E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="P47">
+        <v>48</v>
+      </c>
+      <c r="Q47">
+        <v>8.2994122116360799E-4</v>
+      </c>
+      <c r="T47">
+        <v>48</v>
+      </c>
+      <c r="U47">
+        <v>1.1817599966889201E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="P48">
+        <v>49</v>
+      </c>
+      <c r="Q48">
+        <v>8.3986910933163004E-4</v>
+      </c>
+      <c r="T48">
+        <v>49</v>
+      </c>
+      <c r="U48">
+        <v>1.1917682777857401E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P49">
+        <v>50</v>
+      </c>
+      <c r="Q49">
+        <v>8.6233335721772096E-4</v>
+      </c>
+      <c r="T49">
+        <v>50</v>
+      </c>
+      <c r="U49">
+        <v>1.2285449868068099E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P50">
+        <v>51</v>
+      </c>
+      <c r="Q50">
+        <v>9.5471371256280601E-4</v>
+      </c>
+      <c r="T50">
+        <v>51</v>
+      </c>
+      <c r="U50">
+        <v>1.2964449304854399E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P51">
+        <v>52</v>
+      </c>
+      <c r="Q51">
+        <v>9.2949083016719599E-4</v>
+      </c>
+      <c r="T51">
+        <v>52</v>
+      </c>
+      <c r="U51">
+        <v>1.3668334117392E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P52">
+        <v>53</v>
+      </c>
+      <c r="Q52">
+        <v>1.0122383350971999E-3</v>
+      </c>
+      <c r="T52">
+        <v>53</v>
+      </c>
+      <c r="U52">
+        <v>1.5038183896103801E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P53">
+        <v>54</v>
+      </c>
+      <c r="Q53">
+        <v>1.0357721109176001E-3</v>
+      </c>
+      <c r="T53">
+        <v>54</v>
+      </c>
+      <c r="U53">
+        <v>1.58918501983862E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P54">
+        <v>55</v>
+      </c>
+      <c r="Q54">
+        <v>1.0558746109018101E-3</v>
+      </c>
+      <c r="T54">
+        <v>55</v>
+      </c>
+      <c r="U54">
+        <v>1.62724709080066E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P55">
+        <v>56</v>
+      </c>
+      <c r="Q55">
+        <v>1.05846661375835E-3</v>
+      </c>
+      <c r="T55">
+        <v>56</v>
+      </c>
+      <c r="U55">
+        <v>1.6528599709272299E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P56">
+        <v>57</v>
+      </c>
+      <c r="Q56">
+        <v>1.18077578721567E-3</v>
+      </c>
+      <c r="T56">
+        <v>57</v>
+      </c>
+      <c r="U56">
+        <v>1.68392538907937E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P57">
+        <v>58</v>
+      </c>
+      <c r="Q57">
+        <v>1.19588537723757E-3</v>
+      </c>
+      <c r="T57">
+        <v>58</v>
+      </c>
+      <c r="U57">
+        <v>1.77183706080541E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P58">
+        <v>59</v>
+      </c>
+      <c r="Q58">
+        <v>1.18515375826973E-3</v>
+      </c>
+      <c r="T58">
+        <v>59</v>
+      </c>
+      <c r="U58">
+        <v>1.76879171049222E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P59">
+        <v>60</v>
+      </c>
+      <c r="Q59">
+        <v>1.26816581818275E-3</v>
+      </c>
+      <c r="T59">
+        <v>60</v>
+      </c>
+      <c r="U59">
+        <v>1.8773941445397199E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P60">
+        <v>61</v>
+      </c>
+      <c r="Q60">
+        <v>1.2654233619104999E-3</v>
+      </c>
+      <c r="T60">
+        <v>61</v>
+      </c>
+      <c r="U60">
+        <v>1.90642753033898E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P61">
+        <v>62</v>
+      </c>
+      <c r="Q61">
+        <v>1.2727038102457299E-3</v>
+      </c>
+      <c r="T61">
+        <v>62</v>
+      </c>
+      <c r="U61">
+        <v>1.9269191328203301E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P62">
+        <v>63</v>
+      </c>
+      <c r="Q62">
+        <v>1.3832629215903499E-3</v>
+      </c>
+      <c r="T62">
+        <v>63</v>
+      </c>
+      <c r="U62">
+        <v>1.9956970715429602E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P63">
+        <v>64</v>
+      </c>
+      <c r="Q63">
+        <v>1.3980466709472201E-3</v>
+      </c>
+      <c r="T63">
+        <v>64</v>
+      </c>
+      <c r="U63">
+        <v>2.12817793304566E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P64">
+        <v>65</v>
+      </c>
+      <c r="Q64">
+        <v>1.4034487516619201E-3</v>
+      </c>
+      <c r="T64">
+        <v>65</v>
+      </c>
+      <c r="U64">
+        <v>2.17676497937645E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P65">
+        <v>66</v>
+      </c>
+      <c r="Q65">
+        <v>1.5340858016861601E-3</v>
+      </c>
+      <c r="T65">
+        <v>66</v>
+      </c>
+      <c r="U65">
+        <v>2.21612582099624E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P66">
+        <v>67</v>
+      </c>
+      <c r="Q66">
+        <v>1.54261124960612E-3</v>
+      </c>
+      <c r="T66">
+        <v>67</v>
+      </c>
+      <c r="U66">
+        <v>2.2838545835111202E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P67">
+        <v>68</v>
+      </c>
+      <c r="Q67">
+        <v>1.7340075282845601E-3</v>
+      </c>
+      <c r="T67">
+        <v>68</v>
+      </c>
+      <c r="U67">
+        <v>2.44817168510053E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P68">
+        <v>69</v>
+      </c>
+      <c r="Q68">
+        <v>1.68403745337855E-3</v>
+      </c>
+      <c r="T68">
+        <v>69</v>
+      </c>
+      <c r="U68">
+        <v>2.5572337000630699E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P69">
+        <v>70</v>
+      </c>
+      <c r="Q69">
+        <v>1.66684085328597E-3</v>
+      </c>
+      <c r="T69">
+        <v>70</v>
+      </c>
+      <c r="U69">
+        <v>2.5042536959517699E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P70">
+        <v>71</v>
+      </c>
+      <c r="Q70">
+        <v>1.74656591960228E-3</v>
+      </c>
+      <c r="T70">
+        <v>71</v>
+      </c>
+      <c r="U70">
+        <v>2.5760029058437702E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P71">
+        <v>72</v>
+      </c>
+      <c r="Q71">
+        <v>1.7284537095110799E-3</v>
+      </c>
+      <c r="T71">
+        <v>72</v>
+      </c>
+      <c r="U71">
+        <v>2.6332553592510501E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P72">
+        <v>73</v>
+      </c>
+      <c r="Q72">
+        <v>1.82399500277824E-3</v>
+      </c>
+      <c r="T72">
+        <v>73</v>
+      </c>
+      <c r="U72">
+        <v>2.7335854613920602E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P73">
+        <v>74</v>
+      </c>
+      <c r="Q73">
+        <v>1.84629912138916E-3</v>
+      </c>
+      <c r="T73">
+        <v>74</v>
+      </c>
+      <c r="U73">
+        <v>2.7747900452231898E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P74">
+        <v>75</v>
+      </c>
+      <c r="Q74">
+        <v>1.9146308518247601E-3</v>
+      </c>
+      <c r="T74">
+        <v>75</v>
+      </c>
+      <c r="U74">
+        <v>2.90563798975199E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P75">
+        <v>76</v>
+      </c>
+      <c r="Q75">
+        <v>2.04645336198154E-3</v>
+      </c>
+      <c r="T75">
+        <v>76</v>
+      </c>
+      <c r="U75">
+        <v>3.0648337997263202E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P76">
+        <v>77</v>
+      </c>
+      <c r="Q76">
+        <v>2.0177037484245298E-3</v>
+      </c>
+      <c r="T76">
+        <v>77</v>
+      </c>
+      <c r="U76">
+        <v>3.09652250900398E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P77">
+        <v>78</v>
+      </c>
+      <c r="Q77">
+        <v>2.0009324513375702E-3</v>
+      </c>
+      <c r="T77">
+        <v>78</v>
+      </c>
+      <c r="U77">
+        <v>3.1346241495339199E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P78">
+        <v>79</v>
+      </c>
+      <c r="Q78">
+        <v>2.12167540856171E-3</v>
+      </c>
+      <c r="T78">
+        <v>79</v>
+      </c>
+      <c r="U78">
+        <v>3.2852633495349401E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P79">
+        <v>80</v>
+      </c>
+      <c r="Q79">
+        <v>2.12150918727275E-3</v>
+      </c>
+      <c r="T79">
+        <v>80</v>
+      </c>
+      <c r="U79">
+        <v>3.28628252376802E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P80">
+        <v>81</v>
+      </c>
+      <c r="Q80">
+        <v>2.1680837305029801E-3</v>
+      </c>
+      <c r="T80">
+        <v>81</v>
+      </c>
+      <c r="U80">
+        <v>3.33615830051712E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P81">
+        <v>82</v>
+      </c>
+      <c r="Q81">
+        <v>2.25721295166295E-3</v>
+      </c>
+      <c r="T81">
+        <v>82</v>
+      </c>
+      <c r="U81">
+        <v>3.53150459646713E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P82">
+        <v>83</v>
+      </c>
+      <c r="Q82">
+        <v>2.30503415688872E-3</v>
+      </c>
+      <c r="T82">
+        <v>83</v>
+      </c>
+      <c r="U82">
+        <v>3.4876750211697001E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P83">
+        <v>84</v>
+      </c>
+      <c r="Q83">
+        <v>2.3732678929809401E-3</v>
+      </c>
+      <c r="T83">
+        <v>84</v>
+      </c>
+      <c r="U83">
+        <v>3.6583299515768799E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P84">
+        <v>85</v>
+      </c>
+      <c r="Q84">
+        <v>2.4002895702142199E-3</v>
+      </c>
+      <c r="T84">
+        <v>85</v>
+      </c>
+      <c r="U84">
+        <v>3.70327410928439E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P85">
+        <v>86</v>
+      </c>
+      <c r="Q85">
+        <v>2.4288807890843599E-3</v>
+      </c>
+      <c r="T85">
+        <v>86</v>
+      </c>
+      <c r="U85">
+        <v>3.69138298963662E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P86">
+        <v>87</v>
+      </c>
+      <c r="Q86">
+        <v>2.5841428927378699E-3</v>
+      </c>
+      <c r="T86">
+        <v>87</v>
+      </c>
+      <c r="U86">
+        <v>3.9679799997247699E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P87">
+        <v>88</v>
+      </c>
+      <c r="Q87">
+        <v>2.59344832797069E-3</v>
+      </c>
+      <c r="T87">
+        <v>88</v>
+      </c>
+      <c r="U87">
+        <v>3.9138829743023901E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P88">
+        <v>89</v>
+      </c>
+      <c r="Q88">
+        <v>2.61824251094367E-3</v>
+      </c>
+      <c r="T88">
+        <v>89</v>
+      </c>
+      <c r="U88">
+        <v>4.0904341713758098E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P89">
+        <v>90</v>
+      </c>
+      <c r="Q89">
+        <v>2.7670137392124101E-3</v>
+      </c>
+      <c r="T89">
+        <v>90</v>
+      </c>
+      <c r="U89">
+        <v>4.2132207902613999E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P90">
+        <v>91</v>
+      </c>
+      <c r="Q90">
+        <v>2.69532873120624E-3</v>
+      </c>
+      <c r="T90">
+        <v>91</v>
+      </c>
+      <c r="U90">
+        <v>4.2841654474614103E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P91">
+        <v>92</v>
+      </c>
+      <c r="Q91">
+        <v>2.8988733602454799E-3</v>
+      </c>
+      <c r="T91">
+        <v>92</v>
+      </c>
+      <c r="U91">
+        <v>4.37532620911952E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P92">
+        <v>93</v>
+      </c>
+      <c r="Q92">
+        <v>2.9719525383552501E-3</v>
+      </c>
+      <c r="T92">
+        <v>93</v>
+      </c>
+      <c r="U92">
+        <v>4.6432799898320802E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P93">
+        <v>94</v>
+      </c>
+      <c r="Q93">
+        <v>2.98000418406445E-3</v>
+      </c>
+      <c r="T93">
+        <v>94</v>
+      </c>
+      <c r="U93">
+        <v>4.6054391079815103E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P94">
+        <v>95</v>
+      </c>
+      <c r="Q94">
+        <v>2.9406187293352501E-3</v>
+      </c>
+      <c r="T94">
+        <v>95</v>
+      </c>
+      <c r="U94">
+        <v>4.6528808085713504E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P95">
+        <v>96</v>
+      </c>
+      <c r="Q95">
+        <v>3.04686831776052E-3</v>
+      </c>
+      <c r="T95">
+        <v>96</v>
+      </c>
+      <c r="U95">
+        <v>4.7733304341090804E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P96">
+        <v>97</v>
+      </c>
+      <c r="Q96">
+        <v>3.14345660677645E-3</v>
+      </c>
+      <c r="T96">
+        <v>97</v>
+      </c>
+      <c r="U96">
+        <v>4.8752482858253603E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P97">
+        <v>98</v>
+      </c>
+      <c r="Q97">
+        <v>3.2536904170410701E-3</v>
+      </c>
+      <c r="T97">
+        <v>98</v>
+      </c>
+      <c r="U97">
+        <v>5.0044813490239901E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="16:21" x14ac:dyDescent="0.2">
+      <c r="P98">
+        <v>99</v>
+      </c>
+      <c r="Q98">
+        <v>3.1204191473079802E-3</v>
+      </c>
+      <c r="T98">
+        <v>99</v>
+      </c>
+      <c r="U98">
+        <v>4.83338041813112E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>